<commit_message>
fixed some issues, added yfinance for timeseries daily adjusted
</commit_message>
<xml_diff>
--- a/data/raw/d_quarterly_income_raw.xlsx
+++ b/data/raw/d_quarterly_income_raw.xlsx
@@ -6777,7 +6777,7 @@
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>10895000000</t>
+          <t>11182000000</t>
         </is>
       </c>
       <c r="AA47" t="inlineStr">
@@ -6912,7 +6912,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>14250000000</t>
+          <t>14597000000</t>
         </is>
       </c>
       <c r="AA48" t="inlineStr">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>18798000000</t>
+          <t>19260000000</t>
         </is>
       </c>
       <c r="AA49" t="inlineStr">
@@ -7317,7 +7317,7 @@
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>12408000000</t>
+          <t>12696000000</t>
         </is>
       </c>
       <c r="AA51" t="inlineStr">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>16124000000</t>
+          <t>15384000000</t>
         </is>
       </c>
       <c r="AA52" t="inlineStr">
@@ -9342,7 +9342,7 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>1576000000</t>
+          <t>1442000000</t>
         </is>
       </c>
       <c r="AA66" t="inlineStr">
@@ -9477,7 +9477,7 @@
       </c>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>1509000000</t>
+          <t>1392000000</t>
         </is>
       </c>
       <c r="AA67" t="inlineStr">

</xml_diff>